<commit_message>
made the selector run with real data
</commit_message>
<xml_diff>
--- a/Preliminary_classes/results_caching/results.xlsx
+++ b/Preliminary_classes/results_caching/results.xlsx
@@ -32,6 +32,13 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -39,7 +46,31 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -49,22 +80,6 @@
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -92,14 +107,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
       <charset val="134"/>
       <b val="1"/>
       <color theme="3"/>
@@ -117,6 +124,20 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <b val="1"/>
       <color rgb="FF3F3F3F"/>
       <sz val="11"/>
@@ -125,20 +146,6 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <b val="1"/>
       <color rgb="FFFA7D00"/>
       <sz val="11"/>
@@ -147,13 +154,6 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -162,14 +162,14 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -183,187 +183,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,6 +426,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -440,17 +455,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -463,23 +474,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -497,130 +497,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,13 +1014,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5"/>
   <cols>
     <col width="22.1818181818182" customWidth="1" style="1" min="1" max="1"/>
   </cols>
@@ -1040,11 +1040,33 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>09/11/2022 08:15:55</t>
+          <t>09/11/2022 09:11:29</t>
         </is>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>0.46625</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:16:00</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.47875</v>
       </c>
     </row>
   </sheetData>
@@ -1058,13 +1080,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4"/>
   <cols>
     <col width="24.5454545454545" customWidth="1" style="1" min="1" max="1"/>
   </cols>
@@ -1082,13 +1104,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>09/11/2022 08:15:55</t>
+          <t>09/11/2022 09:11:31</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
+      <c r="B2" s="0" t="n">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:16:03</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.475</v>
       </c>
     </row>
   </sheetData>
@@ -1102,13 +1143,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
   <cols>
     <col width="21.3636363636364" customWidth="1" style="1" min="1" max="1"/>
   </cols>
@@ -1125,6 +1166,26 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:11:50</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.48625</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:16:21</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.4825</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
improved the classification algorithms
</commit_message>
<xml_diff>
--- a/Preliminary_classes/results_caching/results.xlsx
+++ b/Preliminary_classes/results_caching/results.xlsx
@@ -1014,7 +1014,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="$A2:$XFD2"/>
@@ -1069,6 +1069,56 @@
         <v>0.47875</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:28:43</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.545</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:32:53</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.545</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:33:17</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.545</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:35:40</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.545</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:37:12</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.545</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1080,7 +1130,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="$A2:$XFD2"/>
@@ -1132,6 +1182,46 @@
         <v>0.475</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:28:46</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.475</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:33:20</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.58125</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:35:43</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.585</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:37:15</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.585</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1143,7 +1233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="$A1:$XFD1"/>
@@ -1177,13 +1267,43 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>09/11/2022 09:16:21</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="0" t="n">
         <v>0.4825</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:33:39</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.4825</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:36:03</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.4825</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>09/11/2022 09:37:35</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>